<commit_message>
update project list folders
</commit_message>
<xml_diff>
--- a/PMTool16Bit_Core/src/PMTool16Bit.Web.Host/Download/ProjectTasks.xlsx
+++ b/PMTool16Bit_Core/src/PMTool16Bit.Web.Host/Download/ProjectTasks.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="56">
   <si>
     <t xml:space="preserve">Test new project</t>
   </si>
@@ -26,7 +26,7 @@
     <t xml:space="preserve">Sunday, 30 June 2019</t>
   </si>
   <si>
-    <t xml:space="preserve">admin, HoanLeader, </t>
+    <t xml:space="preserve">admin, HoanLeader</t>
   </si>
   <si>
     <t xml:space="preserve">ASDSAA</t>
@@ -44,7 +44,7 @@
     <t xml:space="preserve">jihknmk</t>
   </si>
   <si>
-    <t xml:space="preserve">Saturday, 29 June 2019</t>
+    <t xml:space="preserve">Friday, 30 August 2019</t>
   </si>
   <si>
     <t xml:space="preserve">hbhbjbnjnj</t>
@@ -56,9 +56,6 @@
     <t xml:space="preserve">sadd</t>
   </si>
   <si>
-    <t xml:space="preserve">Tuesday, 25 June 2019</t>
-  </si>
-  <si>
     <t xml:space="preserve">sadsad</t>
   </si>
   <si>
@@ -74,19 +71,13 @@
     <t xml:space="preserve">asd</t>
   </si>
   <si>
-    <t xml:space="preserve">Tuesday, 04 June 2019</t>
-  </si>
-  <si>
     <t xml:space="preserve">assadasd</t>
   </si>
   <si>
     <t xml:space="preserve">dsadasd</t>
   </si>
   <si>
-    <t xml:space="preserve">Wednesday, 12 June 2019</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nobita, </t>
+    <t xml:space="preserve">Nobita</t>
   </si>
   <si>
     <t xml:space="preserve">asdasd</t>
@@ -98,6 +89,9 @@
     <t xml:space="preserve">task122</t>
   </si>
   <si>
+    <t xml:space="preserve">Tuesday, 30 July 2019</t>
+  </si>
+  <si>
     <t xml:space="preserve">1111111</t>
   </si>
   <si>
@@ -113,7 +107,7 @@
     <t xml:space="preserve">232131</t>
   </si>
   <si>
-    <t xml:space="preserve">admin, HoanLeader, HoanTester, </t>
+    <t xml:space="preserve">admin, HoanLeader, HoanTester</t>
   </si>
   <si>
     <t xml:space="preserve">34234234</t>
@@ -131,10 +125,7 @@
     <t xml:space="preserve">12321wwqeqw</t>
   </si>
   <si>
-    <t xml:space="preserve">Thursday, 27 June 2019</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HoanTester, </t>
+    <t xml:space="preserve">HoanTester</t>
   </si>
   <si>
     <t xml:space="preserve">qweqwe</t>
@@ -149,7 +140,7 @@
     <t xml:space="preserve">QWE21</t>
   </si>
   <si>
-    <t xml:space="preserve">HoanLeader, </t>
+    <t xml:space="preserve">HoanLeader</t>
   </si>
   <si>
     <t xml:space="preserve">123213weqwq</t>
@@ -159,6 +150,9 @@
   </si>
   <si>
     <t xml:space="preserve">sdsd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Monday, 17 June 2019</t>
   </si>
   <si>
     <t xml:space="preserve">Project name</t>
@@ -238,8 +232,8 @@
     <col min="1" max="1" width="19.1640625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="20" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="28.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="36.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="25.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="35.1640625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="17.1640625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="10" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="8" max="8" width="13.33203125" bestFit="1" customWidth="1" collapsed="1"/>
@@ -248,31 +242,31 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" t="s">
         <v>49</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>50</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>51</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>52</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>53</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>54</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>55</v>
-      </c>
-      <c r="H1" t="s">
-        <v>56</v>
-      </c>
-      <c r="I1" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="2">
@@ -342,11 +336,11 @@
         <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="E4"/>
       <c r="F4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G4" t="s">
         <v>6</v>
@@ -355,7 +349,7 @@
         <v>6</v>
       </c>
       <c r="I4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5">
@@ -366,14 +360,14 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D5" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E5"/>
       <c r="F5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G5" t="s">
         <v>6</v>
@@ -382,7 +376,7 @@
         <v>6</v>
       </c>
       <c r="I5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6">
@@ -393,14 +387,14 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D6" t="s">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="E6"/>
       <c r="F6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G6" t="s">
         <v>6</v>
@@ -409,7 +403,7 @@
         <v>6</v>
       </c>
       <c r="I6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7">
@@ -420,17 +414,17 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" t="s">
         <v>22</v>
       </c>
-      <c r="D7" t="s">
-        <v>23</v>
-      </c>
-      <c r="E7" t="s">
-        <v>24</v>
-      </c>
-      <c r="F7" t="s">
-        <v>25</v>
-      </c>
       <c r="G7" t="s">
         <v>6</v>
       </c>
@@ -438,7 +432,7 @@
         <v>6</v>
       </c>
       <c r="I7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8">
@@ -446,19 +440,19 @@
         <v>0</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D8" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="E8" t="s">
         <v>4</v>
       </c>
       <c r="F8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G8" t="s">
         <v>7</v>
@@ -467,7 +461,7 @@
         <v>7</v>
       </c>
       <c r="I8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9">
@@ -475,15 +469,17 @@
         <v>0</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C9" t="s">
-        <v>30</v>
-      </c>
-      <c r="D9"/>
+        <v>28</v>
+      </c>
+      <c r="D9" t="s">
+        <v>3</v>
+      </c>
       <c r="E9"/>
       <c r="F9" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G9" t="s">
         <v>6</v>
@@ -492,7 +488,7 @@
         <v>6</v>
       </c>
       <c r="I9" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10">
@@ -500,18 +496,20 @@
         <v>0</v>
       </c>
       <c r="B10" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" t="s">
+        <v>31</v>
+      </c>
+      <c r="F10" t="s">
         <v>32</v>
       </c>
-      <c r="D10"/>
-      <c r="E10" t="s">
-        <v>33</v>
-      </c>
-      <c r="F10" t="s">
-        <v>34</v>
-      </c>
       <c r="G10" t="s">
         <v>6</v>
       </c>
@@ -519,7 +517,7 @@
         <v>6</v>
       </c>
       <c r="I10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11">
@@ -527,15 +525,17 @@
         <v>0</v>
       </c>
       <c r="B11" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C11" t="s">
-        <v>35</v>
-      </c>
-      <c r="D11"/>
+        <v>33</v>
+      </c>
+      <c r="D11" t="s">
+        <v>3</v>
+      </c>
       <c r="E11"/>
       <c r="F11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G11" t="s">
         <v>6</v>
@@ -544,7 +544,7 @@
         <v>6</v>
       </c>
       <c r="I11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12">
@@ -552,20 +552,20 @@
         <v>0</v>
       </c>
       <c r="B12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E12" t="s">
         <v>37</v>
       </c>
-      <c r="C12" t="s">
+      <c r="F12" t="s">
         <v>38</v>
       </c>
-      <c r="D12" t="s">
-        <v>39</v>
-      </c>
-      <c r="E12" t="s">
-        <v>40</v>
-      </c>
-      <c r="F12" t="s">
-        <v>41</v>
-      </c>
       <c r="G12" t="s">
         <v>6</v>
       </c>
@@ -573,7 +573,7 @@
         <v>6</v>
       </c>
       <c r="I12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13">
@@ -581,15 +581,17 @@
         <v>0</v>
       </c>
       <c r="B13" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C13" t="s">
-        <v>42</v>
-      </c>
-      <c r="D13"/>
+        <v>39</v>
+      </c>
+      <c r="D13" t="s">
+        <v>3</v>
+      </c>
       <c r="E13"/>
       <c r="F13" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="G13" t="s">
         <v>6</v>
@@ -598,7 +600,7 @@
         <v>6</v>
       </c>
       <c r="I13" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14">
@@ -606,17 +608,19 @@
         <v>0</v>
       </c>
       <c r="B14" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C14" t="s">
-        <v>44</v>
-      </c>
-      <c r="D14"/>
+        <v>41</v>
+      </c>
+      <c r="D14" t="s">
+        <v>3</v>
+      </c>
       <c r="E14" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F14" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G14" t="s">
         <v>7</v>
@@ -633,15 +637,17 @@
         <v>0</v>
       </c>
       <c r="B15" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C15" t="s">
-        <v>48</v>
-      </c>
-      <c r="D15"/>
+        <v>45</v>
+      </c>
+      <c r="D15" t="s">
+        <v>46</v>
+      </c>
       <c r="E15"/>
       <c r="F15" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="G15" t="s">
         <v>6</v>
@@ -650,7 +656,7 @@
         <v>6</v>
       </c>
       <c r="I15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>